<commit_message>
"Alteração feita em mapeamento e processing para melhor desepenho"
</commit_message>
<xml_diff>
--- a/Processos_20240917131041.xlsx
+++ b/Processos_20240917131041.xlsx
@@ -1,31 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Richard\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33081FA2-4DCE-4501-B7F8-49B0CD4A05F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Planilha1"/>
   </sheets>
   <definedNames>
     <definedName name="HTML_1">Planilha1!$A$1:$AO$103</definedName>
     <definedName name="HTML_all">Planilha1!$A$1:$AO$103</definedName>
     <definedName name="HTML_tables">Planilha1!$A$1:$A$1</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
-    </ext>
-  </extLst>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -3650,23 +3639,28 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3677,7 +3671,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -3689,38 +3690,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="5">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -3747,116 +3753,82 @@
         <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3868,179 +3840,222 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:tint val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:tint val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="9500"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot rev="0" lon="0" lat="0"/>
+            </a:camera>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:tint val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:AO121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="11.5546875"/>
+    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="34" max="34" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="35" max="35" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="36" max="36" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="37" max="37" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="38" max="38" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="39" max="39" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="40" max="40" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="41" max="41" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4165,7 +4180,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="2" t="s">
         <v>41</v>
       </c>
@@ -4290,7 +4305,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="2" t="s">
         <v>65</v>
       </c>
@@ -4415,7 +4430,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="2" t="s">
         <v>79</v>
       </c>
@@ -4540,7 +4555,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="2" t="s">
         <v>90</v>
       </c>
@@ -4665,7 +4680,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="2" t="s">
         <v>103</v>
       </c>
@@ -4790,7 +4805,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="2" t="s">
         <v>114</v>
       </c>
@@ -4915,7 +4930,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="2" t="s">
         <v>123</v>
       </c>
@@ -5040,7 +5055,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="2" t="s">
         <v>133</v>
       </c>
@@ -5165,7 +5180,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="2" t="s">
         <v>142</v>
       </c>
@@ -5290,7 +5305,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="2" t="s">
         <v>151</v>
       </c>
@@ -5415,7 +5430,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="2" t="s">
         <v>158</v>
       </c>
@@ -5540,7 +5555,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="2" t="s">
         <v>168</v>
       </c>
@@ -5665,7 +5680,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="2" t="s">
         <v>180</v>
       </c>
@@ -5790,7 +5805,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="2" t="s">
         <v>191</v>
       </c>
@@ -5915,7 +5930,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="2" t="s">
         <v>201</v>
       </c>
@@ -6040,7 +6055,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="2" t="s">
         <v>212</v>
       </c>
@@ -6165,7 +6180,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="2" t="s">
         <v>219</v>
       </c>
@@ -6290,7 +6305,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="2" t="s">
         <v>234</v>
       </c>
@@ -6415,7 +6430,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="2" t="s">
         <v>243</v>
       </c>
@@ -6540,7 +6555,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="2" t="s">
         <v>253</v>
       </c>
@@ -6665,7 +6680,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="2" t="s">
         <v>261</v>
       </c>
@@ -6790,7 +6805,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="2" t="s">
         <v>269</v>
       </c>
@@ -6915,7 +6930,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="2" t="s">
         <v>278</v>
       </c>
@@ -7040,7 +7055,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="2" t="s">
         <v>287</v>
       </c>
@@ -7165,7 +7180,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="2" t="s">
         <v>295</v>
       </c>
@@ -7290,7 +7305,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="2" t="s">
         <v>305</v>
       </c>
@@ -7415,7 +7430,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="2" t="s">
         <v>314</v>
       </c>
@@ -7540,7 +7555,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="2" t="s">
         <v>326</v>
       </c>
@@ -7665,7 +7680,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="2" t="s">
         <v>335</v>
       </c>
@@ -7790,7 +7805,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="2" t="s">
         <v>348</v>
       </c>
@@ -7915,7 +7930,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="2" t="s">
         <v>361</v>
       </c>
@@ -8040,7 +8055,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="2" t="s">
         <v>371</v>
       </c>
@@ -8165,7 +8180,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="2" t="s">
         <v>383</v>
       </c>
@@ -8290,7 +8305,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="2" t="s">
         <v>395</v>
       </c>
@@ -8415,7 +8430,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="2" t="s">
         <v>406</v>
       </c>
@@ -8540,7 +8555,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
       <c r="A37" s="2" t="s">
         <v>416</v>
       </c>
@@ -8665,7 +8680,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="2" t="s">
         <v>426</v>
       </c>
@@ -8790,7 +8805,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
       <c r="A39" s="2" t="s">
         <v>435</v>
       </c>
@@ -8915,7 +8930,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="40" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
       <c r="A40" s="2" t="s">
         <v>450</v>
       </c>
@@ -9040,7 +9055,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="41" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
       <c r="A41" s="2" t="s">
         <v>462</v>
       </c>
@@ -9165,7 +9180,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="42" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
       <c r="A42" s="2" t="s">
         <v>473</v>
       </c>
@@ -9290,7 +9305,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
       <c r="A43" s="2" t="s">
         <v>482</v>
       </c>
@@ -9415,7 +9430,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="44" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
       <c r="A44" s="2" t="s">
         <v>491</v>
       </c>
@@ -9540,7 +9555,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="45" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
       <c r="A45" s="2" t="s">
         <v>295</v>
       </c>
@@ -9665,7 +9680,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="46" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
       <c r="A46" s="2" t="s">
         <v>507</v>
       </c>
@@ -9790,7 +9805,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
       <c r="A47" s="2" t="s">
         <v>519</v>
       </c>
@@ -9915,7 +9930,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="48" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
       <c r="A48" s="2" t="s">
         <v>535</v>
       </c>
@@ -10040,7 +10055,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="49" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
       <c r="A49" s="2" t="s">
         <v>547</v>
       </c>
@@ -10165,7 +10180,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="50" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
       <c r="A50" s="2" t="s">
         <v>557</v>
       </c>
@@ -10290,7 +10305,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="51" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
       <c r="A51" s="2" t="s">
         <v>567</v>
       </c>
@@ -10415,7 +10430,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="52" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
       <c r="A52" s="2" t="s">
         <v>581</v>
       </c>
@@ -10540,7 +10555,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
       <c r="A53" s="2" t="s">
         <v>592</v>
       </c>
@@ -10665,7 +10680,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="54" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
       <c r="A54" s="2" t="s">
         <v>605</v>
       </c>
@@ -10790,7 +10805,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="55" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
       <c r="A55" s="2" t="s">
         <v>614</v>
       </c>
@@ -10915,7 +10930,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="56" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
       <c r="A56" s="2" t="s">
         <v>621</v>
       </c>
@@ -11040,7 +11055,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="57" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
       <c r="A57" s="2" t="s">
         <v>634</v>
       </c>
@@ -11165,7 +11180,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="58" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
       <c r="A58" s="2" t="s">
         <v>649</v>
       </c>
@@ -11290,7 +11305,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="59" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
       <c r="A59" s="2" t="s">
         <v>662</v>
       </c>
@@ -11415,7 +11430,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="60" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
       <c r="A60" s="2" t="s">
         <v>676</v>
       </c>
@@ -11540,7 +11555,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="61" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
       <c r="A61" s="2" t="s">
         <v>687</v>
       </c>
@@ -11665,7 +11680,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="62" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
       <c r="A62" s="2" t="s">
         <v>702</v>
       </c>
@@ -11790,7 +11805,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="63" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
       <c r="A63" s="2" t="s">
         <v>716</v>
       </c>
@@ -11875,7 +11890,7 @@
       <c r="AB63" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AC63" s="2"/>
+      <c r="AC63" s="3"/>
       <c r="AD63" s="2" t="s">
         <v>62</v>
       </c>
@@ -11913,7 +11928,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="64" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
       <c r="A64" s="2" t="s">
         <v>721</v>
       </c>
@@ -12038,7 +12053,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="65" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
       <c r="A65" s="2" t="s">
         <v>733</v>
       </c>
@@ -12163,7 +12178,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="66" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
       <c r="A66" s="2" t="s">
         <v>743</v>
       </c>
@@ -12288,7 +12303,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="67" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
       <c r="A67" s="2" t="s">
         <v>757</v>
       </c>
@@ -12373,7 +12388,7 @@
       <c r="AB67" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AC67" s="2"/>
+      <c r="AC67" s="3"/>
       <c r="AD67" s="2" t="s">
         <v>62</v>
       </c>
@@ -12411,7 +12426,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="68" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
       <c r="A68" s="2" t="s">
         <v>762</v>
       </c>
@@ -12496,7 +12511,7 @@
       <c r="AB68" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AC68" s="2"/>
+      <c r="AC68" s="3"/>
       <c r="AD68" s="2" t="s">
         <v>62</v>
       </c>
@@ -12534,7 +12549,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="69" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
       <c r="A69" s="2" t="s">
         <v>766</v>
       </c>
@@ -12659,7 +12674,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="70" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
       <c r="A70" s="2" t="s">
         <v>775</v>
       </c>
@@ -12784,7 +12799,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="71" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
       <c r="A71" s="2" t="s">
         <v>790</v>
       </c>
@@ -12909,7 +12924,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="72" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
       <c r="A72" s="2" t="s">
         <v>797</v>
       </c>
@@ -13034,7 +13049,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="73" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
       <c r="A73" s="2" t="s">
         <v>808</v>
       </c>
@@ -13159,7 +13174,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="74" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
       <c r="A74" s="2" t="s">
         <v>818</v>
       </c>
@@ -13284,7 +13299,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="75" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
       <c r="A75" s="2" t="s">
         <v>833</v>
       </c>
@@ -13409,7 +13424,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="76" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
       <c r="A76" s="2" t="s">
         <v>847</v>
       </c>
@@ -13534,7 +13549,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="77" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
       <c r="A77" s="2" t="s">
         <v>853</v>
       </c>
@@ -13659,7 +13674,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="78" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
       <c r="A78" s="2" t="s">
         <v>863</v>
       </c>
@@ -13784,7 +13799,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="79" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
       <c r="A79" s="2" t="s">
         <v>872</v>
       </c>
@@ -13909,7 +13924,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="80" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
       <c r="A80" s="2" t="s">
         <v>883</v>
       </c>
@@ -13994,7 +14009,7 @@
       <c r="AB80" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AC80" s="2"/>
+      <c r="AC80" s="3"/>
       <c r="AD80" s="2" t="s">
         <v>62</v>
       </c>
@@ -14032,7 +14047,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="81" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
       <c r="A81" s="2" t="s">
         <v>886</v>
       </c>
@@ -14117,7 +14132,7 @@
       <c r="AB81" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AC81" s="2"/>
+      <c r="AC81" s="3"/>
       <c r="AD81" s="2" t="s">
         <v>890</v>
       </c>
@@ -14155,7 +14170,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="82" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
       <c r="A82" s="2" t="s">
         <v>892</v>
       </c>
@@ -14240,7 +14255,7 @@
       <c r="AB82" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AC82" s="2"/>
+      <c r="AC82" s="3"/>
       <c r="AD82" s="2" t="s">
         <v>62</v>
       </c>
@@ -14278,7 +14293,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="83" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
       <c r="A83" s="2" t="s">
         <v>896</v>
       </c>
@@ -14403,7 +14418,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="84" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
       <c r="A84" s="2" t="s">
         <v>907</v>
       </c>
@@ -14528,7 +14543,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="85" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
       <c r="A85" s="2" t="s">
         <v>916</v>
       </c>
@@ -14653,7 +14668,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="86" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
       <c r="A86" s="2" t="s">
         <v>923</v>
       </c>
@@ -14778,7 +14793,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="87" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
       <c r="A87" s="2" t="s">
         <v>931</v>
       </c>
@@ -14863,7 +14878,7 @@
       <c r="AB87" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AC87" s="2"/>
+      <c r="AC87" s="3"/>
       <c r="AD87" s="2" t="s">
         <v>62</v>
       </c>
@@ -14901,7 +14916,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="88" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
       <c r="A88" s="2" t="s">
         <v>935</v>
       </c>
@@ -15026,7 +15041,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="89" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
       <c r="A89" s="2" t="s">
         <v>941</v>
       </c>
@@ -15151,7 +15166,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="90" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
       <c r="A90" s="2" t="s">
         <v>951</v>
       </c>
@@ -15276,7 +15291,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="91" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
       <c r="A91" s="2" t="s">
         <v>960</v>
       </c>
@@ -15401,7 +15416,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="92" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
       <c r="A92" s="2" t="s">
         <v>971</v>
       </c>
@@ -15526,7 +15541,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="93" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
       <c r="A93" s="2" t="s">
         <v>981</v>
       </c>
@@ -15651,7 +15666,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="94" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
       <c r="A94" s="2" t="s">
         <v>993</v>
       </c>
@@ -15776,7 +15791,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="95" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
       <c r="A95" s="2" t="s">
         <v>998</v>
       </c>
@@ -15901,7 +15916,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="96" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
       <c r="A96" s="2" t="s">
         <v>1008</v>
       </c>
@@ -16026,7 +16041,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="97" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
       <c r="A97" s="2" t="s">
         <v>1019</v>
       </c>
@@ -16151,7 +16166,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="98" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
       <c r="A98" s="2" t="s">
         <v>1028</v>
       </c>
@@ -16276,7 +16291,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="99" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
       <c r="A99" s="2" t="s">
         <v>1041</v>
       </c>
@@ -16401,7 +16416,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="100" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
       <c r="A100" s="2" t="s">
         <v>1051</v>
       </c>
@@ -16526,7 +16541,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="101" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75">
       <c r="A101" s="2" t="s">
         <v>1057</v>
       </c>
@@ -16651,7 +16666,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="102" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75">
       <c r="A102" s="2" t="s">
         <v>1068</v>
       </c>
@@ -16776,7 +16791,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="103" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75">
       <c r="A103" s="2" t="s">
         <v>1079</v>
       </c>
@@ -16901,7 +16916,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="104" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75">
       <c r="A104" s="2" t="s">
         <v>1085</v>
       </c>
@@ -17026,7 +17041,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="105" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75">
       <c r="A105" s="2" t="s">
         <v>1093</v>
       </c>
@@ -17151,7 +17166,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="106" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18.75">
       <c r="A106" s="2" t="s">
         <v>1103</v>
       </c>
@@ -17276,7 +17291,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="107" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75">
       <c r="A107" s="2" t="s">
         <v>1110</v>
       </c>
@@ -17401,7 +17416,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="108" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75">
       <c r="A108" s="2" t="s">
         <v>1121</v>
       </c>
@@ -17486,7 +17501,7 @@
       <c r="AB108" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AC108" s="2"/>
+      <c r="AC108" s="3"/>
       <c r="AD108" s="2" t="s">
         <v>890</v>
       </c>
@@ -17524,7 +17539,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="109" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18.75">
       <c r="A109" s="2" t="s">
         <v>1125</v>
       </c>
@@ -17649,7 +17664,7 @@
         <v>1137</v>
       </c>
     </row>
-    <row r="110" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18.75">
       <c r="A110" s="2" t="s">
         <v>1138</v>
       </c>
@@ -17734,7 +17749,7 @@
       <c r="AB110" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AC110" s="2"/>
+      <c r="AC110" s="3"/>
       <c r="AD110" s="2" t="s">
         <v>62</v>
       </c>
@@ -17772,7 +17787,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="111" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18.75">
       <c r="A111" s="2" t="s">
         <v>1141</v>
       </c>
@@ -17857,7 +17872,7 @@
       <c r="AB111" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AC111" s="2"/>
+      <c r="AC111" s="3"/>
       <c r="AD111" s="2" t="s">
         <v>155</v>
       </c>
@@ -17895,7 +17910,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="112" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18.75">
       <c r="A112" s="2" t="s">
         <v>1147</v>
       </c>
@@ -17980,7 +17995,7 @@
       <c r="AB112" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AC112" s="2"/>
+      <c r="AC112" s="3"/>
       <c r="AD112" s="2" t="s">
         <v>479</v>
       </c>
@@ -18018,7 +18033,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="113" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18.75">
       <c r="A113" s="2" t="s">
         <v>1150</v>
       </c>
@@ -18103,7 +18118,7 @@
       <c r="AB113" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AC113" s="2"/>
+      <c r="AC113" s="3"/>
       <c r="AD113" s="2" t="s">
         <v>1153</v>
       </c>
@@ -18141,7 +18156,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="114" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18.75">
       <c r="A114" s="2" t="s">
         <v>1156</v>
       </c>
@@ -18266,7 +18281,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="115" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="18.75">
       <c r="A115" s="2" t="s">
         <v>1165</v>
       </c>
@@ -18391,7 +18406,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="116" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="18.75">
       <c r="A116" s="2" t="s">
         <v>1171</v>
       </c>
@@ -18476,7 +18491,7 @@
       <c r="AB116" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AC116" s="2"/>
+      <c r="AC116" s="3"/>
       <c r="AD116" s="2" t="s">
         <v>155</v>
       </c>
@@ -18514,7 +18529,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="117" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="18.75">
       <c r="A117" s="2" t="s">
         <v>1174</v>
       </c>
@@ -18599,7 +18614,7 @@
       <c r="AB117" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AC117" s="2"/>
+      <c r="AC117" s="3"/>
       <c r="AD117" s="2" t="s">
         <v>155</v>
       </c>
@@ -18637,7 +18652,7 @@
         <v>1179</v>
       </c>
     </row>
-    <row r="118" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="18.75">
       <c r="A118" s="2" t="s">
         <v>1180</v>
       </c>
@@ -18722,7 +18737,7 @@
       <c r="AB118" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AC118" s="2"/>
+      <c r="AC118" s="3"/>
       <c r="AD118" s="2" t="s">
         <v>155</v>
       </c>
@@ -18760,7 +18775,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="119" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="18.75">
       <c r="A119" s="2" t="s">
         <v>1183</v>
       </c>
@@ -18845,7 +18860,7 @@
       <c r="AB119" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AC119" s="2"/>
+      <c r="AC119" s="3"/>
       <c r="AD119" s="2" t="s">
         <v>155</v>
       </c>
@@ -18883,7 +18898,7 @@
         <v>1187</v>
       </c>
     </row>
-    <row r="120" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="18.75">
       <c r="A120" s="2" t="s">
         <v>1188</v>
       </c>
@@ -19008,7 +19023,7 @@
         <v>1196</v>
       </c>
     </row>
-    <row r="121" spans="1:41" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="18.75">
       <c r="A121" s="2" t="s">
         <v>1197</v>
       </c>
@@ -19134,11 +19149,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>